<commit_message>
update Xray-Normal Schablone: Ergebnisse aus den Tests eingebaut
</commit_message>
<xml_diff>
--- a/Schablonen/XrayNormal_alt.xlsx
+++ b/Schablonen/XrayNormal_alt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92720E49-7CD7-4836-9283-C3931F2A30D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85081613-6DEA-4A95-A44A-905C0CDD215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61320" yWindow="6690" windowWidth="29040" windowHeight="15720" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="448">
   <si>
     <t>Gliederung</t>
   </si>
@@ -277,9 +277,6 @@
     <t>2. Shaldon-Katheter</t>
   </si>
   <si>
-    <t>2. Shaldon-Katheter;weiterer Shaldon;weiterer Shaldon Katheter;zweiter Shaldon Katheter;zweiter Shaldon</t>
-  </si>
-  <si>
     <t>I10</t>
   </si>
   <si>
@@ -481,21 +478,12 @@
     <t>Klappen-OP;ACB, ACVB</t>
   </si>
   <si>
-    <t>Klappen OP, HK OP;ACB, ACVB</t>
-  </si>
-  <si>
     <t>mit ...</t>
   </si>
   <si>
     <t>Postoperativer Status [nach %I33%. ]</t>
   </si>
   <si>
-    <t>Klappen-OP</t>
-  </si>
-  <si>
-    <t>Klappen OP;Klappen-OP;Herzklappen-OP;Herzklappen OP</t>
-  </si>
-  <si>
     <t>I34</t>
   </si>
   <si>
@@ -550,9 +538,6 @@
     <t>gering</t>
   </si>
   <si>
-    <t>PE gering; geringer PE</t>
-  </si>
-  <si>
     <t>PE1</t>
   </si>
   <si>
@@ -580,9 +565,6 @@
     <t>mäßig</t>
   </si>
   <si>
-    <t>PE mäßig; mäßiger PE</t>
-  </si>
-  <si>
     <t>PE3</t>
   </si>
   <si>
@@ -598,9 +580,6 @@
     <t>deutlich</t>
   </si>
   <si>
-    <t>PE deutlich; deutlicher PE</t>
-  </si>
-  <si>
     <t>PE5</t>
   </si>
   <si>
@@ -655,9 +634,6 @@
     <t>apikal / lateral / basal / ventral / mantelförmig</t>
   </si>
   <si>
-    <t>aperal/lateral/basal/ventral/mantelförmig</t>
-  </si>
-  <si>
     <t>P3</t>
   </si>
   <si>
@@ -883,9 +859,6 @@
     <t>H1</t>
   </si>
   <si>
-    <t>ZahlBruch</t>
-  </si>
-  <si>
     <t>beträgt</t>
   </si>
   <si>
@@ -946,9 +919,6 @@
     <t>Grad 1</t>
   </si>
   <si>
-    <t>Grad 1;pv Stau Grad 1;pv Stau 1;Grad I</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pulmonalvenöse Umverteilung mit dilatierten, scharf begrenzten Oberlappengefäßen (vaskuläre Kranialisation) und normalem Lungeninterstitium. </t>
   </si>
   <si>
@@ -958,9 +928,6 @@
     <t>Grad 2</t>
   </si>
   <si>
-    <t>Grad 2;pv Stau Grad 2;pv Stau 2;Grad II</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mäßige Hypervolämie mit dilatierten, unscharf begrenzten Oberlappengefäßen und Bronchialmanschettenzeichen. </t>
   </si>
   <si>
@@ -970,9 +937,6 @@
     <t>Grad 3</t>
   </si>
   <si>
-    <t>Grad 3;pv Stau Grad 3;pv Stau 3;Grad III</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deutliche Hypervolämie mit zentral unscharf begrenzten Lungengefäßen, Bronchialmanschettenzeichen und vermehrter interstitieller Zeichnung einschließlich Kerley-Linien (interstitielles Lungenödem). </t>
   </si>
   <si>
@@ -982,9 +946,6 @@
     <t>Grad 4</t>
   </si>
   <si>
-    <t>Grad 4;pv Stau Grad 4;pv Stau 4;Grad IV</t>
-  </si>
-  <si>
     <t xml:space="preserve">Massive Hypervolämie mit zentral und peripher unscharf abgrenzbaren Lungengefäßen sowie deutlich vermehrt interstitieller und fleckförmiger Zeichnung (interstitelles und alveoläres Lungenödem). </t>
   </si>
   <si>
@@ -1189,9 +1150,6 @@
     <t>Z.n. CHE</t>
   </si>
   <si>
-    <t>CHE;Cholezystektomie;Cholecystektomie</t>
-  </si>
-  <si>
     <t xml:space="preserve">Z.n. CHE bei entsprechend projizierten OP-Clips im li. OB. </t>
   </si>
   <si>
@@ -1240,9 +1198,6 @@
     <t>WT-Emphysem</t>
   </si>
   <si>
-    <t>Weichteil Emphysem;WT Emphysem</t>
-  </si>
-  <si>
     <t>W1</t>
   </si>
   <si>
@@ -1261,9 +1216,6 @@
     <t>weiteres WT-Emphysem</t>
   </si>
   <si>
-    <t>weiteres Weichteil Emphysem;weiteres WT Emphysem</t>
-  </si>
-  <si>
     <t>W4</t>
   </si>
   <si>
@@ -1376,6 +1328,57 @@
   </si>
   <si>
     <t>Variable-Default</t>
+  </si>
+  <si>
+    <t>2. Shaldon-Katheter;weiterer Shaldon;weiterer Shaldon Katheter;zweiter Shaldon Katheter;zweiter Shaldon;2. Shaldon</t>
+  </si>
+  <si>
+    <t>FAL;freie abdominelle Luft</t>
+  </si>
+  <si>
+    <t>CHE;Cholezystektomie;Cholecystektomie;Z.n. CHE</t>
+  </si>
+  <si>
+    <t>PE gering; geringer PE;Pleuraerguss gering; geringer Pleuraerguss</t>
+  </si>
+  <si>
+    <t>PE mäßig; mäßiger PE;Pleuraerguss mäßig;mäßiger Pleuraerguss</t>
+  </si>
+  <si>
+    <t>PE deutlich; deutlicher PE;Pleuraerguss deutlich; deutlicher Pleuraerguss</t>
+  </si>
+  <si>
+    <t>Klappen-OP;ACB, ACVB;ACB;ACVB</t>
+  </si>
+  <si>
+    <t>kein PE;kein Pleuraerguss</t>
+  </si>
+  <si>
+    <t>Art der Klappen-OP</t>
+  </si>
+  <si>
+    <t>Art der Klappen-OP;Art der Klappen OP</t>
+  </si>
+  <si>
+    <t>apikal/lateral/basal/ventral/mantelförmig</t>
+  </si>
+  <si>
+    <t>pv Stau Grad 1;pv Stau 1;pv Stau Grad eins</t>
+  </si>
+  <si>
+    <t>pv Stau Grad 2;pv Stau 2;pv Stau Grad zwei</t>
+  </si>
+  <si>
+    <t>pv Stau Grad 3;pv Stau 3;pv Stau Grad drei</t>
+  </si>
+  <si>
+    <t>pv Stau Grad 4;pv Stau 4;pv Stau Grad vier</t>
+  </si>
+  <si>
+    <t>Weichteil Emphysem;WT Emphysem;Weichteileemphysem;Weichteilemphysem</t>
+  </si>
+  <si>
+    <t>weiteres Weichteil Emphysem;weiteres WT Emphysem;weiteres Weichteileemphysem;weiteres Weichteilemphysem</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1456,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1469,7 +1472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1767,32 +1770,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD863459-8DC2-4F08-8B8A-0734853F8245}">
   <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" customWidth="1"/>
-    <col min="11" max="11" width="29.26953125" customWidth="1"/>
-    <col min="12" max="12" width="38.26953125" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" customWidth="1"/>
+    <col min="12" max="12" width="38.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="54" customWidth="1"/>
-    <col min="16" max="16" width="48.453125" customWidth="1"/>
+    <col min="16" max="16" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1830,7 +1833,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -1842,7 +1845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1872,7 +1875,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1898,7 +1901,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1924,7 +1927,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1954,7 +1957,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1986,7 +1989,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -2012,7 +2015,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -2038,7 +2041,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -2070,14 +2073,14 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
@@ -2096,7 +2099,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2118,7 +2121,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -2148,7 +2151,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -2180,7 +2183,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2204,7 +2207,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2228,7 +2231,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
@@ -2260,7 +2263,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2284,7 +2287,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2308,7 +2311,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -2340,7 +2343,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2364,7 +2367,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2388,14 +2391,14 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>431</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2403,7 +2406,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>57</v>
@@ -2416,11 +2419,11 @@
         <v>59</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2431,7 +2434,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>62</v>
@@ -2444,7 +2447,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2455,7 +2458,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>65</v>
@@ -2468,14 +2471,14 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2483,7 +2486,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>57</v>
@@ -2496,11 +2499,11 @@
         <v>59</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2511,7 +2514,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>65</v>
@@ -2524,14 +2527,14 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2539,7 +2542,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>57</v>
@@ -2552,11 +2555,11 @@
         <v>59</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2567,7 +2570,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>65</v>
@@ -2580,14 +2583,14 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2595,7 +2598,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>57</v>
@@ -2608,11 +2611,11 @@
         <v>59</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2623,7 +2626,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>65</v>
@@ -2636,14 +2639,14 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2651,7 +2654,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>57</v>
@@ -2664,11 +2667,11 @@
         <v>59</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2679,7 +2682,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>65</v>
@@ -2692,14 +2695,14 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2707,7 +2710,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>65</v>
@@ -2718,18 +2721,18 @@
       <c r="M33" s="2"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2737,7 +2740,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>65</v>
@@ -2748,18 +2751,18 @@
       <c r="M34" s="2"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2767,7 +2770,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>65</v>
@@ -2778,18 +2781,18 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2797,7 +2800,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>65</v>
@@ -2808,11 +2811,11 @@
       <c r="M36" s="2"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2823,27 +2826,27 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2851,7 +2854,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>57</v>
@@ -2864,11 +2867,11 @@
         <v>59</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2879,20 +2882,20 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2903,27 +2906,27 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2931,22 +2934,22 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2957,7 +2960,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>57</v>
@@ -2972,7 +2975,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2983,22 +2986,22 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="L43" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3009,27 +3012,27 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3037,31 +3040,31 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="L45" s="1" t="s">
-        <v>148</v>
+        <v>437</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>151</v>
+        <v>439</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>152</v>
+        <v>440</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3069,29 +3072,29 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3099,22 +3102,22 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3125,20 +3128,20 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -3156,20 +3159,20 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>166</v>
+        <v>438</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>15</v>
@@ -3178,7 +3181,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -3186,47 +3189,47 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>171</v>
+        <v>434</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3237,54 +3240,54 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="1"/>
       <c r="O52" s="5"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>181</v>
+        <v>435</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3295,54 +3298,54 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="5"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>187</v>
+        <v>436</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3353,20 +3356,20 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="5"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>47</v>
       </c>
@@ -3384,29 +3387,29 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3416,47 +3419,47 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3467,20 +3470,20 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>206</v>
+        <v>441</v>
       </c>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3491,54 +3494,54 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3549,20 +3552,20 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3573,39 +3576,39 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>57</v>
@@ -3616,13 +3619,13 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3633,20 +3636,20 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3657,22 +3660,22 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>47</v>
       </c>
@@ -3690,20 +3693,20 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>15</v>
@@ -3712,7 +3715,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -3720,28 +3723,28 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>57</v>
@@ -3751,52 +3754,52 @@
       </c>
       <c r="M70" s="1"/>
       <c r="N70" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3805,7 +3808,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -3814,20 +3817,20 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>15</v>
@@ -3836,7 +3839,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3844,27 +3847,27 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -3872,27 +3875,27 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -3900,49 +3903,49 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="M76" s="1"/>
       <c r="N76" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3953,36 +3956,36 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -3992,23 +3995,23 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -4018,25 +4021,25 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -4046,23 +4049,23 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="P80" s="1"/>
     </row>
-    <row r="81" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -4072,18 +4075,18 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="P81" s="1"/>
     </row>
-    <row r="82" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -4091,22 +4094,22 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>282</v>
+        <v>119</v>
       </c>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>47</v>
       </c>
@@ -4124,27 +4127,27 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -4154,23 +4157,23 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -4180,23 +4183,23 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -4206,27 +4209,27 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -4236,25 +4239,25 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>303</v>
+        <v>442</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -4264,25 +4267,25 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>307</v>
+        <v>443</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -4292,25 +4295,25 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>311</v>
+        <v>444</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -4320,25 +4323,25 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>315</v>
+        <v>445</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -4348,15 +4351,15 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4365,7 +4368,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -4374,28 +4377,28 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="P92" s="1"/>
     </row>
-    <row r="93" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -4404,24 +4407,24 @@
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="P93" s="1"/>
     </row>
-    <row r="94" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -4430,24 +4433,24 @@
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="P94" s="1"/>
     </row>
-    <row r="95" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -4456,22 +4459,22 @@
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4479,24 +4482,24 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4507,20 +4510,20 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
     </row>
-    <row r="98" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4531,27 +4534,27 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4559,24 +4562,24 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4587,34 +4590,34 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -4624,47 +4627,47 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4675,20 +4678,20 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4699,54 +4702,54 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
     </row>
-    <row r="105" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -4757,20 +4760,20 @@
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
       <c r="J106" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4781,20 +4784,20 @@
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -4805,32 +4808,32 @@
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
       <c r="J108" s="1" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
     </row>
-    <row r="109" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
@@ -4840,13 +4843,13 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -4864,20 +4867,20 @@
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="P110" s="1"/>
     </row>
-    <row r="111" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>15</v>
@@ -4886,7 +4889,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
       <c r="I111" s="1" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -4894,25 +4897,25 @@
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="P111" s="1"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>384</v>
+        <v>433</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
       <c r="I112" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -4920,25 +4923,25 @@
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
       <c r="I113" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -4946,49 +4949,49 @@
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
       <c r="I114" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M114" s="1"/>
       <c r="N114" s="1" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>47</v>
       </c>
@@ -5006,20 +5009,20 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="P115" s="1"/>
     </row>
-    <row r="116" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>15</v>
@@ -5028,7 +5031,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
       <c r="I116" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -5036,45 +5039,45 @@
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="P116" s="1"/>
     </row>
-    <row r="117" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>401</v>
+        <v>446</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
       <c r="I117" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -5085,20 +5088,20 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="1" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -5109,37 +5112,37 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="1" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
       <c r="P119" s="1"/>
     </row>
-    <row r="120" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
       <c r="I120" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="K120" s="1" t="s">
         <v>57</v>
@@ -5150,13 +5153,13 @@
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -5167,20 +5170,20 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="1" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -5191,20 +5194,20 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="1" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
       <c r="P122" s="1"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>47</v>
       </c>
@@ -5222,13 +5225,13 @@
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="P123" s="1"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -5237,7 +5240,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
@@ -5246,22 +5249,22 @@
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="P124" s="1"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>15</v>
@@ -5276,75 +5279,75 @@
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="P125" s="1"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="I126" s="1"/>
       <c r="J126" s="1" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L126" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="P126" s="1"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="P127" s="1"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -5355,52 +5358,52 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="1" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L128" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
       <c r="P128" s="1"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="I129" s="1"/>
       <c r="J129" s="1" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="P129" s="1"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -5411,27 +5414,27 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="1" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5439,26 +5442,26 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="1" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="O131" s="1" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -5469,15 +5472,15 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="1" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
       <c r="N132" s="1" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
@@ -5488,6 +5491,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B662EE53BAED864D9E45A03F917DD171" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0b478698d34ba6ea8d28dcb235cef59d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac726c7a-29b1-4eed-9efa-e398fb837db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bae4f718acc166ce461856f4d6d984a" ns3:_="">
     <xsd:import namespace="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
@@ -5633,22 +5651,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC27FD34-7D59-4F13-870A-01667C34E6ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1CA99AA-BB55-4566-A33D-E268FF599705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5664,28 +5691,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC27FD34-7D59-4F13-870A-01667C34E6ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed parsingError 4 and fixed RöntgenNormal with new rules
</commit_message>
<xml_diff>
--- a/Schablonen/XrayNormal_alt.xlsx
+++ b/Schablonen/XrayNormal_alt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85081613-6DEA-4A95-A44A-905C0CDD215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E0887F-960B-490D-A9D5-055721E004E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
+    <workbookView xWindow="-28920" yWindow="2160" windowWidth="29040" windowHeight="15720" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,9 +664,6 @@
     <t>gering/mäßig/deutlich</t>
   </si>
   <si>
-    <t>Mediastinalshift</t>
-  </si>
-  <si>
     <t>Spannungspneumothorax</t>
   </si>
   <si>
@@ -859,9 +856,6 @@
     <t>H1</t>
   </si>
   <si>
-    <t>beträgt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Die Herz-Thorax-Relation beträgt %H1%. </t>
   </si>
   <si>
@@ -1168,9 +1162,6 @@
     <t>O1</t>
   </si>
   <si>
-    <t xml:space="preserve">Lokalisation FAL </t>
-  </si>
-  <si>
     <t xml:space="preserve">Miterfasste FAL %O1% subdiaphragmal im OB. </t>
   </si>
   <si>
@@ -1379,6 +1370,15 @@
   </si>
   <si>
     <t>weiteres Weichteil Emphysem;weiteres WT Emphysem;weiteres Weichteileemphysem;weiteres Weichteilemphysem</t>
+  </si>
+  <si>
+    <t>Mediastinalshift …</t>
+  </si>
+  <si>
+    <t>beträgt …</t>
+  </si>
+  <si>
+    <t>Lokalisation FAL …</t>
   </si>
 </sst>
 </file>
@@ -1771,18 +1771,19 @@
   <dimension ref="A1:P132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
+      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="6" width="7" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
@@ -1812,7 +1813,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1833,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -2077,10 +2078,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
@@ -2398,7 +2399,7 @@
         <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3046,7 +3047,7 @@
         <v>146</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1" t="s">
@@ -3061,10 +3062,10 @@
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3172,7 +3173,7 @@
         <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>15</v>
@@ -3202,7 +3203,7 @@
         <v>166</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3260,7 +3261,7 @@
         <v>175</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3318,7 +3319,7 @@
         <v>180</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3476,7 +3477,7 @@
         <v>198</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
@@ -3586,7 +3587,7 @@
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="1" t="s">
-        <v>209</v>
+        <v>445</v>
       </c>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -3595,10 +3596,10 @@
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -3608,7 +3609,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>57</v>
@@ -3619,10 +3620,10 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="P65" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="P65" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3636,7 +3637,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>119</v>
@@ -3660,7 +3661,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>207</v>
@@ -3670,7 +3671,7 @@
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="1" t="s">
-        <v>209</v>
+        <v>445</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -3693,20 +3694,20 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P68" s="1"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="P68" s="1"/>
-    </row>
-    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>15</v>
@@ -3715,7 +3716,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -3723,7 +3724,7 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P69" s="1"/>
     </row>
@@ -3731,20 +3732,20 @@
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>57</v>
@@ -3754,10 +3755,10 @@
       </c>
       <c r="M70" s="1"/>
       <c r="N70" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O70" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="P70" s="1"/>
     </row>
@@ -3765,41 +3766,41 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J71" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K71" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="L71" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="O71" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="O71" s="1" t="s">
+      <c r="P71" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="P71" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3808,7 +3809,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -3817,20 +3818,20 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="P72" s="1"/>
+    </row>
+    <row r="73" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="P72" s="1"/>
-    </row>
-    <row r="73" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>15</v>
@@ -3839,7 +3840,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3847,7 +3848,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P73" s="1"/>
     </row>
@@ -3855,19 +3856,19 @@
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -3875,7 +3876,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P74" s="1"/>
     </row>
@@ -3883,19 +3884,19 @@
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -3903,7 +3904,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P75" s="1"/>
     </row>
@@ -3911,38 +3912,38 @@
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J76" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K76" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="M76" s="1"/>
       <c r="N76" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O76" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="O76" s="1" t="s">
+      <c r="P76" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="P76" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -3956,7 +3957,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>119</v>
@@ -3964,28 +3965,28 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -3995,7 +3996,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P78" s="1"/>
     </row>
@@ -4003,15 +4004,15 @@
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -4021,25 +4022,25 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="P79" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="P79" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -4049,7 +4050,7 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P80" s="1"/>
     </row>
@@ -4057,15 +4058,15 @@
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -4075,7 +4076,7 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P81" s="1"/>
     </row>
@@ -4083,10 +4084,10 @@
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -4094,7 +4095,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>119</v>
@@ -4102,10 +4103,10 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1" t="s">
-        <v>274</v>
+        <v>446</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P82" s="1"/>
     </row>
@@ -4127,27 +4128,27 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P83" s="1"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -4157,7 +4158,7 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P84" s="1"/>
     </row>
@@ -4165,15 +4166,15 @@
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -4183,7 +4184,7 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="P85" s="1"/>
     </row>
@@ -4191,15 +4192,15 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -4209,27 +4210,27 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="P86" s="1"/>
     </row>
     <row r="87" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -4239,25 +4240,25 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -4267,25 +4268,25 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -4295,25 +4296,25 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -4323,25 +4324,25 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -4351,15 +4352,15 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4368,7 +4369,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -4377,28 +4378,28 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P92" s="1"/>
     </row>
     <row r="93" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -4407,7 +4408,7 @@
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="P93" s="1"/>
     </row>
@@ -4415,16 +4416,16 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -4433,7 +4434,7 @@
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P94" s="1"/>
     </row>
@@ -4441,16 +4442,16 @@
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -4459,22 +4460,22 @@
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P95" s="1"/>
     </row>
     <row r="96" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4482,21 +4483,21 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L96" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="K96" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="L96" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -4510,7 +4511,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>193</v>
@@ -4534,13 +4535,13 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="L98" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="K98" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="L98" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
@@ -4551,10 +4552,10 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4562,7 +4563,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K99" s="1" t="s">
         <v>193</v>
@@ -4573,10 +4574,10 @@
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -4590,13 +4591,13 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="L100" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="K100" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
@@ -4607,17 +4608,17 @@
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -4627,30 +4628,30 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="102" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>193</v>
@@ -4661,10 +4662,10 @@
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="103" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -4678,13 +4679,13 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="L103" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="K103" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="L103" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
@@ -4702,13 +4703,13 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L104" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="L104" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
@@ -4719,34 +4720,34 @@
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="P105" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="O105" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="P105" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -4760,7 +4761,7 @@
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
       <c r="J106" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>119</v>
@@ -4768,7 +4769,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
@@ -4784,15 +4785,15 @@
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
@@ -4808,15 +4809,15 @@
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
       <c r="J108" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
@@ -4825,15 +4826,15 @@
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
@@ -4843,10 +4844,10 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -4867,20 +4868,20 @@
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P110" s="1"/>
     </row>
-    <row r="111" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>15</v>
@@ -4889,7 +4890,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
       <c r="I111" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -4897,7 +4898,7 @@
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="P111" s="1"/>
     </row>
@@ -4905,17 +4906,17 @@
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
       <c r="I112" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -4923,7 +4924,7 @@
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="P112" s="1"/>
     </row>
@@ -4931,17 +4932,17 @@
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
       <c r="I113" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -4949,30 +4950,30 @@
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
       <c r="I114" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>193</v>
@@ -4982,13 +4983,13 @@
       </c>
       <c r="M114" s="1"/>
       <c r="N114" s="1" t="s">
-        <v>377</v>
+        <v>447</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -5009,20 +5010,20 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="P115" s="1"/>
     </row>
-    <row r="116" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>15</v>
@@ -5031,7 +5032,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
       <c r="I116" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -5039,7 +5040,7 @@
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="P116" s="1"/>
     </row>
@@ -5047,20 +5048,20 @@
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
       <c r="I117" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>193</v>
@@ -5071,10 +5072,10 @@
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -5088,10 +5089,10 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>208</v>
@@ -5112,7 +5113,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>173</v>
@@ -5129,20 +5130,20 @@
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
       <c r="I120" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K120" s="1" t="s">
         <v>57</v>
@@ -5153,10 +5154,10 @@
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
@@ -5170,10 +5171,10 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>208</v>
@@ -5194,7 +5195,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K122" s="1" t="s">
         <v>173</v>
@@ -5225,13 +5226,13 @@
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="P123" s="1"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -5240,7 +5241,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
@@ -5249,22 +5250,22 @@
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="P124" s="1"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>15</v>
@@ -5279,7 +5280,7 @@
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="P125" s="1"/>
     </row>
@@ -5287,20 +5288,20 @@
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I126" s="1"/>
       <c r="J126" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>207</v>
@@ -5311,7 +5312,7 @@
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P126" s="1"/>
     </row>
@@ -5319,20 +5320,20 @@
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>193</v>
@@ -5343,7 +5344,7 @@
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="P127" s="1"/>
     </row>
@@ -5358,7 +5359,7 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>207</v>
@@ -5375,20 +5376,20 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I129" s="1"/>
       <c r="J129" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K129" s="1" t="s">
         <v>193</v>
@@ -5399,7 +5400,7 @@
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="P129" s="1"/>
     </row>
@@ -5414,7 +5415,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="K130" s="1" t="s">
         <v>207</v>
@@ -5431,10 +5432,10 @@
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5442,23 +5443,23 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="O131" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
@@ -5472,15 +5473,15 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
       <c r="N132" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
@@ -5491,21 +5492,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B662EE53BAED864D9E45A03F917DD171" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0b478698d34ba6ea8d28dcb235cef59d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac726c7a-29b1-4eed-9efa-e398fb837db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bae4f718acc166ce461856f4d6d984a" ns3:_="">
     <xsd:import namespace="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
@@ -5651,31 +5637,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC27FD34-7D59-4F13-870A-01667C34E6ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1CA99AA-BB55-4566-A33D-E268FF599705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5691,4 +5668,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC27FD34-7D59-4F13-870A-01667C34E6ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>